<commit_message>
update made january 24th
</commit_message>
<xml_diff>
--- a/100000-120000.xlsx
+++ b/100000-120000.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>CVR</t>
   </si>
@@ -76,6 +76,15 @@
     <t>14194711</t>
   </si>
   <si>
+    <t>34391513</t>
+  </si>
+  <si>
+    <t>10613779</t>
+  </si>
+  <si>
+    <t>66328511</t>
+  </si>
+  <si>
     <t>BPO Visma Løn og HR</t>
   </si>
   <si>
@@ -134,6 +143,9 @@
   </si>
   <si>
     <t>2023Q3</t>
+  </si>
+  <si>
+    <t>2023Q4</t>
   </si>
   <si>
     <t>100000-120000</t>
@@ -498,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -544,19 +556,19 @@
         <v>118122.86</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2">
         <v>44315</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -570,19 +582,19 @@
         <v>101094.66</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2">
         <v>44314</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -596,19 +608,19 @@
         <v>109548</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2">
         <v>44344</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -622,19 +634,19 @@
         <v>109791.88</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E5" s="2">
         <v>44347</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -648,19 +660,19 @@
         <v>117341</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2">
         <v>44462</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -674,19 +686,19 @@
         <v>113561</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2">
         <v>44643</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -700,19 +712,19 @@
         <v>108824</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" s="2">
         <v>44816</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -726,22 +738,22 @@
         <v>101508</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2">
         <v>44875</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -755,16 +767,16 @@
         <v>110646</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2">
         <v>45047</v>
       </c>
       <c r="H10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -778,16 +790,16 @@
         <v>104340</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2">
         <v>45070</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -801,16 +813,88 @@
         <v>100068</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E12" s="2">
         <v>45113</v>
       </c>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I12" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>2023</v>
+      </c>
+      <c r="C13">
+        <v>102035.85</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="2">
+        <v>45196</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>2023</v>
+      </c>
+      <c r="C14">
+        <v>116715</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2">
+        <v>45212</v>
+      </c>
+      <c r="H14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>2023</v>
+      </c>
+      <c r="C15">
+        <v>109559.83</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="2">
+        <v>45245</v>
+      </c>
+      <c r="H15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>